<commit_message>
port battle calculator: format
</commit_message>
<xml_diff>
--- a/src/port-battle.xlsx
+++ b/src/port-battle.xlsx
@@ -219,7 +219,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="6f6150"/>
+      <color rgb="6b7478"/>
     </font>
     <font>
       <b/>
@@ -247,6 +247,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="e9f1f4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="dcc6a9"/>
       </patternFill>
     </fill>
@@ -262,12 +267,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="f3f7f9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="f5efe7"/>
+        <fgColor rgb="ede1d2"/>
       </patternFill>
     </fill>
   </fills>
@@ -306,27 +306,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">

</xml_diff>

<commit_message>
port battle calculator corrected
Former-commit-id: 13976c24740850d1ed6d364eb97ba41b58b508ba
</commit_message>
<xml_diff>
--- a/src/port-battle.xlsx
+++ b/src/port-battle.xlsx
@@ -155,34 +155,37 @@
     <t>Mortar Brig</t>
   </si>
   <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>NavyBrig</t>
+  </si>
+  <si>
+    <t>Niagara</t>
+  </si>
+  <si>
+    <t>Prince de Neufchatel</t>
+  </si>
+  <si>
+    <t>Rattlesnake</t>
+  </si>
+  <si>
+    <t>Rattlesnake Heavy</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
     <t>Brig</t>
   </si>
   <si>
-    <t>Rattlesnake Heavy</t>
-  </si>
-  <si>
-    <t>Mercury</t>
-  </si>
-  <si>
-    <t>NavyBrig</t>
-  </si>
-  <si>
-    <t>Niagara</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>Prince de Neufchatel</t>
-  </si>
-  <si>
-    <t>Rattlesnake</t>
-  </si>
-  <si>
-    <t>Hercules</t>
-  </si>
-  <si>
-    <t>Pandora</t>
+    <t>Pickle</t>
   </si>
   <si>
     <t>Cutter</t>
@@ -201,9 +204,6 @@
   </si>
   <si>
     <t>Yacht Silver</t>
-  </si>
-  <si>
-    <t>Pickle</t>
   </si>
 </sst>
 </file>
@@ -733,10 +733,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="9">
-        <f>SUM(D4:D34)</f>
+        <f>SUM(D4:D35)</f>
       </c>
       <c r="E3" s="9">
-        <f>SUM(E4:E34)</f>
+        <f>SUM(E4:E35)</f>
       </c>
       <c r="F3" s="10" t="s">
         <v>9</v>
@@ -2180,10 +2180,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="9">
-        <f>SUM(D4:D20)</f>
+        <f>SUM(D4:D21)</f>
       </c>
       <c r="E3" s="9">
-        <f>SUM(E4:E20)</f>
+        <f>SUM(E4:E21)</f>
       </c>
       <c r="F3" s="10" t="s">
         <v>9</v>
@@ -2200,7 +2200,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="12">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D4" s="12">
         <f t="shared" ref="D4:D21" si="0">COUNTIF(F4:AE4,"*")</f>
@@ -2248,7 +2248,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="12">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="0"/>
@@ -2590,7 +2590,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="12">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" si="0"/>
@@ -2632,7 +2632,7 @@
         <v>56</v>
       </c>
       <c r="C14" s="12">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" si="0"/>
@@ -2674,7 +2674,7 @@
         <v>57</v>
       </c>
       <c r="C15" s="12">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" si="0"/>
@@ -2926,7 +2926,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="12">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D21" s="12">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
port battle calculator: "0" not displayed
Former-commit-id: ece8486d65395abaa76bd2f745ee9e76d828dcbd
</commit_message>
<xml_diff>
--- a/src/port-battle.xlsx
+++ b/src/port-battle.xlsx
@@ -210,6 +210,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <color theme="1"/>
@@ -296,18 +299,18 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -316,14 +319,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">

</xml_diff>

<commit_message>
tweet updates: n/a as nation if not in tweets
Former-commit-id: e4aa192e5db2cb9edaa8d2463052ce992f0cbd7d [formerly 8db7d588da8e7a6f8b44dd4f8a1a8f9d8f9180d2]
Former-commit-id: 2a0666d10a266f5fcb87c2a2cfd7f98e8eeef82a
</commit_message>
<xml_diff>
--- a/src/port-battle.xlsx
+++ b/src/port-battle.xlsx
@@ -1354,7 +1354,7 @@
     <numFmt formatCode="#" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1391,6 +1391,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFE7E8DE"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="1"/>
       <b/>
@@ -1469,20 +1476,20 @@
   </borders>
   <cellXfs count="35">
     <xf applyFont="1" fontId="0"/>
-    <xf applyBorder="1" borderId="1"/>
+    <xf applyFont="1" fontId="0" applyBorder="1" borderId="1"/>
     <xf applyFont="1" fontId="1"/>
-    <xf applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
-    <xf applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="2"/>
     <xf applyFont="1" fontId="2" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="2"/>
-    <xf applyFont="1" fontId="2" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="2"/>
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="3" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
@@ -1492,57 +1499,57 @@
     <xf applyFont="1" fontId="4" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="2" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="2" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="5"/>
     <xf applyFont="1" fontId="5" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="3"/>
-    <xf applyFont="1" fontId="5" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="3"/>
+    <xf applyFont="1" fontId="6" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="5" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
-      <alignment horizontal="right" indent="1" vertical="center"/>
-    </xf>
-    <xf applyFont="1" fontId="6"/>
     <xf applyFont="1" fontId="6" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="4"/>
+    <xf applyFont="1" fontId="7"/>
+    <xf applyFont="1" fontId="7" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+      <alignment horizontal="right" indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="4"/>
     <xf applyFont="1" fontId="6" applyFill="1" fillId="4" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="4" applyFill="1" fillId="3" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="7"/>
-    <xf applyFont="1" fontId="7" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="8"/>
+    <xf applyFont="1" fontId="8" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="7" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="2" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="2" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="2" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="2" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="5"/>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="5" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="5"/>
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="5" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="6"/>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="6" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="6"/>
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="6" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="6" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="6" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
-    <xf applyFill="1" fillId="7"/>
-    <xf applyFont="1" fontId="7" applyFill="1" fillId="7" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="7"/>
+    <xf applyFont="1" fontId="0" applyFill="1" fillId="7" applyBorder="1" borderId="1" applyNumberFormat="1" numFmtId="165" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6662,7 +6669,7 @@
         <v>369</v>
       </c>
       <c r="C21" s="27" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D21" s="27">
         <f>COUNTA(F21:AC21)</f>
@@ -6709,7 +6716,7 @@
         <v>370</v>
       </c>
       <c r="C22" s="27" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D22" s="27">
         <f>COUNTA(F22:AC22)</f>

</xml_diff>

<commit_message>
patch 27: building-list corrected
</commit_message>
<xml_diff>
--- a/src/port-battle.xlsx
+++ b/src/port-battle.xlsx
@@ -59,10 +59,10 @@
     <t>Victory</t>
   </si>
   <si>
+    <t>Bucentaure</t>
+  </si>
+  <si>
     <t>Christian</t>
-  </si>
-  <si>
-    <t>Bucentaure</t>
   </si>
   <si>
     <t>St. Pavel</t>
@@ -1947,7 +1947,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="32" t="n">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="D8" s="32">
         <f>COUNTA(F8:AC8)</f>
@@ -1994,7 +1994,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="32" t="n">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D9" s="32">
         <f>COUNTA(F9:AC9)</f>

</xml_diff>